<commit_message>
Finalized features to add every week's list
</commit_message>
<xml_diff>
--- a/Trello Backlog Dispatcher/BoardList.xlsx
+++ b/Trello Backlog Dispatcher/BoardList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\Trello Backlog Dispatcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E42D97-A14C-44B4-A8B8-2AE810A524C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A025AD57-9D0F-4487-B45B-561E4528C5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="8115" windowWidth="28185" windowHeight="11265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="6180" windowWidth="28185" windowHeight="11265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,13 @@
     <t>Board Name</t>
   </si>
   <si>
-    <t>Andrew Shields-Java Foundations Project</t>
+    <t>Andrew Shields - Java Foundations Project</t>
   </si>
   <si>
-    <t>Marielle Nolasco-.NET Foundations Project</t>
+    <t>Moiya Josephs - Java Foundations Project</t>
   </si>
   <si>
-    <t>Moiya Josephs-Java Foundations Project</t>
+    <t>Marielle Nolasco - .NET Foundations Project</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -409,12 +409,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>